<commit_message>
ui stuff and updates for card
</commit_message>
<xml_diff>
--- a/server/UFC_Trackrecord.xlsx
+++ b/server/UFC_Trackrecord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ay3xqa\AlexYu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633AB265-0FFB-4412-81E6-D3E519519B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B63854-4473-4D38-9E25-D0782384A167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3600" windowWidth="21600" windowHeight="11700" xr2:uid="{D9C141C5-5A16-4075-9E7D-7275F87CF902}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D9C141C5-5A16-4075-9E7D-7275F87CF902}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -144,16 +144,55 @@
   </si>
   <si>
     <t>Virna Jandiroba</t>
+  </si>
+  <si>
+    <t>UFC 304: Edwards vs. Muhammad 2</t>
+  </si>
+  <si>
+    <t>Arnold Allen</t>
+  </si>
+  <si>
+    <t>Giga Chikadze</t>
+  </si>
+  <si>
+    <t>Muhammad Mokaev</t>
+  </si>
+  <si>
+    <t>Manel Kape</t>
+  </si>
+  <si>
+    <t>King Green</t>
+  </si>
+  <si>
+    <t>Paddy Pimblett</t>
+  </si>
+  <si>
+    <t>Tom Aspinall</t>
+  </si>
+  <si>
+    <t>Curtis Blaydes</t>
+  </si>
+  <si>
+    <t>Leon Edwards</t>
+  </si>
+  <si>
+    <t>Belal Muhammad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -517,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13D26B7-331A-437C-9652-B7D95D2D3849}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,8 +569,8 @@
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -555,10 +594,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -587,10 +626,10 @@
         <v>2.5</v>
       </c>
       <c r="F2">
+        <v>-145</v>
+      </c>
+      <c r="G2">
         <v>114</v>
-      </c>
-      <c r="G2">
-        <v>-145</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -619,10 +658,10 @@
         <v>1.5</v>
       </c>
       <c r="F3">
+        <v>-166</v>
+      </c>
+      <c r="G3">
         <v>130</v>
-      </c>
-      <c r="G3">
-        <v>-166</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -652,10 +691,10 @@
         <v>1.5</v>
       </c>
       <c r="F4">
+        <v>-135</v>
+      </c>
+      <c r="G4">
         <v>105</v>
-      </c>
-      <c r="G4">
-        <v>-135</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
@@ -684,10 +723,10 @@
         <v>2.5</v>
       </c>
       <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
         <v>-130</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -716,10 +755,10 @@
         <v>4.5</v>
       </c>
       <c r="F6">
+        <v>-315</v>
+      </c>
+      <c r="G6">
         <v>230</v>
-      </c>
-      <c r="G6">
-        <v>-315</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
@@ -748,10 +787,10 @@
         <v>2.5</v>
       </c>
       <c r="F7">
+        <v>-105</v>
+      </c>
+      <c r="G7">
         <v>-125</v>
-      </c>
-      <c r="G7">
-        <v>-105</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -780,10 +819,10 @@
         <v>2.5</v>
       </c>
       <c r="F8">
+        <v>-188</v>
+      </c>
+      <c r="G8">
         <v>145</v>
-      </c>
-      <c r="G8">
-        <v>-188</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -812,10 +851,10 @@
         <v>2.5</v>
       </c>
       <c r="F9">
+        <v>-200</v>
+      </c>
+      <c r="G9">
         <v>154</v>
-      </c>
-      <c r="G9">
-        <v>-200</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
@@ -845,10 +884,10 @@
         <v>2.5</v>
       </c>
       <c r="F10">
+        <v>105</v>
+      </c>
+      <c r="G10">
         <v>-135</v>
-      </c>
-      <c r="G10">
-        <v>105</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
@@ -877,10 +916,10 @@
         <v>2.5</v>
       </c>
       <c r="F11">
+        <v>150</v>
+      </c>
+      <c r="G11">
         <v>-195</v>
-      </c>
-      <c r="G11">
-        <v>150</v>
       </c>
       <c r="H11" t="s">
         <v>13</v>
@@ -909,10 +948,10 @@
         <v>2.5</v>
       </c>
       <c r="F12">
+        <v>-175</v>
+      </c>
+      <c r="G12">
         <v>135</v>
-      </c>
-      <c r="G12">
-        <v>-175</v>
       </c>
       <c r="H12" t="s">
         <v>13</v>
@@ -924,7 +963,177 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45500</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13">
+        <v>2.5</v>
+      </c>
+      <c r="F13">
+        <v>-245</v>
+      </c>
+      <c r="G13">
+        <v>185</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13">
+        <f>100/245</f>
+        <v>0.40816326530612246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45500</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>2.5</v>
+      </c>
+      <c r="F14">
+        <v>-238</v>
+      </c>
+      <c r="G14">
+        <v>180</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <f>100/238</f>
+        <v>0.42016806722689076</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45500</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15">
+        <v>2.5</v>
+      </c>
+      <c r="F15">
+        <v>-188</v>
+      </c>
+      <c r="G15">
+        <v>145</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45500</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <v>1.5</v>
+      </c>
+      <c r="F16">
+        <v>135</v>
+      </c>
+      <c r="G16">
+        <v>-175</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <f>100/175</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45500</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17">
+        <v>4.5</v>
+      </c>
+      <c r="F17">
+        <v>-230</v>
+      </c>
+      <c r="G17">
+        <v>175</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>